<commit_message>
code backup before pull
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/databrain-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/databrain-api-engine-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E4DD81-9626-4E62-970C-12FFEA32A76B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C093C4E7-2953-4329-AF9C-2EB54231E92D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDataGraphQL" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
   <si>
     <t>description</t>
   </si>
@@ -50,9 +50,6 @@
   </si>
   <si>
     <t>rspCode</t>
-  </si>
-  <si>
-    <t>explain</t>
   </si>
   <si>
     <t>{ValueDetails(cond:"{id: {_eq: \"System1:GmsDevice_1_7210_4194307.Present_Value\"}}")  {DataType ErrorCode id Value ObjectId PropertyName AttributeId IsArray}}</t>
@@ -167,6 +164,21 @@
     "condition": "id='1'",
     "name": "Floor"
 }</t>
+  </si>
+  <si>
+    <t>databrain-getDataGraphQL-test-1</t>
+  </si>
+  <si>
+    <t>good request, data retrieved</t>
+  </si>
+  <si>
+    <t>{AM100 {tvoc activity illumination co2 temperature infrared_and_visible humidity infrared pressure deviceName devEUI}}</t>
+  </si>
+  <si>
+    <t>databrain-getDataGraphQL-test-2</t>
+  </si>
+  <si>
+    <t>{VS121 {stime people_counter_all deviceName devEUI}}</t>
   </si>
 </sst>
 </file>
@@ -248,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -261,6 +273,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -542,25 +557,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB954454-8325-44B2-8EFC-770E32FDCBE2}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.77734375" style="2" customWidth="1"/>
     <col min="2" max="2" width="35.77734375" style="2" customWidth="1"/>
     <col min="3" max="3" width="73.44140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="2"/>
+    <col min="7" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -568,7 +582,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
@@ -579,11 +593,49 @@
       <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>5</v>
+    </row>
+    <row r="2" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="5">
+        <v>200</v>
+      </c>
+      <c r="E2" s="5">
+        <v>100000</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="5">
+        <v>200</v>
+      </c>
+      <c r="E3" s="5">
+        <v>100000</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -593,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE22B0A1-EDF6-487D-8C5B-FE5F049504FE}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -623,22 +675,22 @@
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>2</v>
@@ -650,32 +702,32 @@
         <v>3</v>
       </c>
       <c r="L1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="I2" s="1">
         <v>200</v>
@@ -684,31 +736,31 @@
         <v>100000</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I3" s="1">
         <v>200</v>
@@ -717,31 +769,31 @@
         <v>100000</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:13" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="I4" s="1">
         <v>200</v>
@@ -750,32 +802,32 @@
         <v>100000</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="1:13" ht="234.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1">
@@ -785,7 +837,7 @@
         <v>100000</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L5" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
update test cases for data-brain-test
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/databrain-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/databrain-api-engine-test-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C093C4E7-2953-4329-AF9C-2EB54231E92D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6237FE2-BB1E-491B-BA1A-493792D5347C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
   <si>
     <t>description</t>
   </si>
@@ -179,6 +179,9 @@
   </si>
   <si>
     <t>{VS121 {stime people_counter_all deviceName devEUI}}</t>
+  </si>
+  <si>
+    <t>query</t>
   </si>
 </sst>
 </file>
@@ -560,7 +563,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -582,7 +585,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
re add test case for sdl-7869
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/databrain-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/databrain-api-engine-test-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-backup\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB15882D-2BD7-4DAD-9C6C-907B09EB4199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716DF40A-5559-48A6-AD1C-64CCDA70D3AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDataGraphQL" sheetId="6" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="129">
   <si>
     <t>description</t>
   </si>
@@ -494,7 +494,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -503,7 +503,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Calibri"/>
+        <rFont val="等线"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -3760,43 +3760,96 @@
   <si>
     <t>反控空调模式</t>
   </si>
+  <si>
+    <t>databrain-getDataGraphQL-test-3</t>
+  </si>
+  <si>
+    <t>{Equipment {type sourceId description _isPartOf id name}}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Successfully</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>databrain-getDataGraphQL-test-4</t>
+  </si>
+  <si>
+    <t>{Location {type sourceId description _isPartOf id name}}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>databrain-getDataGraphQL-test-5</t>
+  </si>
+  <si>
+    <t>{Point {sourceId sourceSystem type id description _isPointOf name}}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>databrain-getDataGraphQL-test-6</t>
+  </si>
+  <si>
+    <t>{Sensor {sourceId sourceSystem type id description _isPointOf name}}</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>databrain-getDataGraphQL-test-11</t>
+  </si>
+  <si>
+    <t>{Humidity_Sensor {sourceId sourceSystem type id description _isPointOf name isPointOf_Thermostat {type sourceId description _isPartOf id name}}}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>databrain-getDataGraphQL-test-12</t>
+  </si>
+  <si>
+    <t>{Room {type sourceId description _isPartOf id name isPartOf_Floor {type sourceId description _isPartOf id name}}}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -4150,13 +4203,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13585E94-2A3C-423F-8526-0CA62361FED2}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" style="2" bestFit="1" customWidth="1"/>
@@ -4167,7 +4220,7 @@
     <col min="7" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -4187,7 +4240,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>35</v>
       </c>
@@ -4207,7 +4260,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
@@ -4227,7 +4280,128 @@
         <v>7</v>
       </c>
     </row>
+    <row r="4" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" s="2">
+        <v>200</v>
+      </c>
+      <c r="E4" s="2">
+        <v>100000</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" s="2">
+        <v>200</v>
+      </c>
+      <c r="E5" s="2">
+        <v>100000</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6" s="2">
+        <v>200</v>
+      </c>
+      <c r="E6" s="2">
+        <v>100000</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" s="2">
+        <v>200</v>
+      </c>
+      <c r="E7" s="2">
+        <v>100000</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D8" s="2">
+        <v>200</v>
+      </c>
+      <c r="E8" s="2">
+        <v>100000</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D9" s="2">
+        <v>200</v>
+      </c>
+      <c r="E9" s="2">
+        <v>100000</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4241,7 +4415,7 @@
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.33203125" style="2" bestFit="1" customWidth="1"/>
@@ -4259,7 +4433,7 @@
     <col min="14" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -4300,7 +4474,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -4333,7 +4507,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -4366,7 +4540,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -4399,7 +4573,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" ht="234.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="224.4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -4447,11 +4621,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70680153-503C-4505-8AE3-05CAD87026D8}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.77734375" style="2" bestFit="1" customWidth="1"/>
@@ -4464,7 +4638,7 @@
     <col min="9" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -4490,7 +4664,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>44</v>
       </c>
@@ -4516,7 +4690,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>48</v>
       </c>
@@ -4542,7 +4716,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>52</v>
       </c>
@@ -4568,7 +4742,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>56</v>
       </c>
@@ -4594,7 +4768,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>60</v>
       </c>
@@ -4620,7 +4794,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>64</v>
       </c>
@@ -4640,7 +4814,7 @@
       </c>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>66</v>
       </c>
@@ -4666,7 +4840,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>71</v>
       </c>
@@ -4692,7 +4866,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>75</v>
       </c>
@@ -4718,7 +4892,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>80</v>
       </c>
@@ -4744,7 +4918,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>84</v>
       </c>
@@ -4770,7 +4944,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>88</v>
       </c>
@@ -4796,7 +4970,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>91</v>
       </c>
@@ -4822,7 +4996,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>94</v>
       </c>
@@ -4848,7 +5022,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>98</v>
       </c>
@@ -4874,7 +5048,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>102</v>
       </c>
@@ -4898,7 +5072,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>106</v>
       </c>
@@ -4922,7 +5096,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>108</v>
       </c>
@@ -4946,7 +5120,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>110</v>
       </c>
@@ -4970,7 +5144,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>112</v>
       </c>
@@ -4994,7 +5168,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="67.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>114</v>
       </c>

</xml_diff>

<commit_message>
add test cases for smart space
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/databrain-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/databrain-api-engine-test-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB6A5CA-FED8-4F90-B580-A15628486FB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50A4B4D6-5688-404C-86C5-B2249184CD37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDataGraphQL" sheetId="6" r:id="rId1"/>
@@ -1249,7 +1249,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13585E94-2A3C-423F-8526-0CA62361FED2}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -1334,13 +1334,13 @@
       <c r="C4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="2">
-        <v>200</v>
-      </c>
-      <c r="E4" s="2">
-        <v>100000</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="D4" s="1">
+        <v>200</v>
+      </c>
+      <c r="E4" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1351,16 +1351,16 @@
       <c r="B5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="2">
-        <v>200</v>
-      </c>
-      <c r="E5" s="2">
-        <v>100000</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="D5" s="1">
+        <v>200</v>
+      </c>
+      <c r="E5" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1371,16 +1371,16 @@
       <c r="B6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="2">
-        <v>200</v>
-      </c>
-      <c r="E6" s="2">
-        <v>100000</v>
-      </c>
-      <c r="F6" s="2" t="s">
+      <c r="D6" s="1">
+        <v>200</v>
+      </c>
+      <c r="E6" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1391,16 +1391,16 @@
       <c r="B7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D7" s="2">
-        <v>200</v>
-      </c>
-      <c r="E7" s="2">
-        <v>100000</v>
-      </c>
-      <c r="F7" s="2" t="s">
+      <c r="D7" s="1">
+        <v>200</v>
+      </c>
+      <c r="E7" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1411,16 +1411,16 @@
       <c r="B8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D8" s="2">
-        <v>200</v>
-      </c>
-      <c r="E8" s="2">
-        <v>100000</v>
-      </c>
-      <c r="F8" s="2" t="s">
+      <c r="D8" s="1">
+        <v>200</v>
+      </c>
+      <c r="E8" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1431,16 +1431,16 @@
       <c r="B9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="2">
-        <v>200</v>
-      </c>
-      <c r="E9" s="2">
-        <v>100000</v>
-      </c>
-      <c r="F9" s="2" t="s">
+      <c r="D9" s="1">
+        <v>200</v>
+      </c>
+      <c r="E9" s="1">
+        <v>100000</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1456,7 +1456,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8"/>
@@ -1665,8 +1665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70680153-503C-4505-8AE3-05CAD87026D8}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8"/>

</xml_diff>

<commit_message>
delete desigoCC/enlighted/MQTT test cases in databrain-prod
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/databrain-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/databrain-api-engine-test-data.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EFDC281-AC09-4E23-AE0B-72D1EE0B9A9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0267038D-EE06-497C-91CE-ACEDD18C4B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="getDataGraphQL" sheetId="6" r:id="rId1"/>
+    <sheet name="getDataGraphQL-bc" sheetId="6" r:id="rId1"/>
     <sheet name="queryUpdateFromApiEngine" sheetId="3" r:id="rId2"/>
     <sheet name="verifySmartSpaceWenSiQueryFunc" sheetId="7" r:id="rId3"/>
     <sheet name="verifySmartSpacePropertyFunc" sheetId="8" r:id="rId4"/>
@@ -9250,8 +9250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13585E94-2A3C-423F-8526-0CA62361FED2}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8"/>
@@ -9666,7 +9666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{441672E3-2DED-4E9A-92CB-8665FC4F9165}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add test cases for story SDL-8913
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/databrain-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/databrain-api-engine-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0267038D-EE06-497C-91CE-ACEDD18C4B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A22C9C-B90B-4DC7-87F4-2E16881B6650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDataGraphQL-bc" sheetId="6" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="730">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="729">
   <si>
     <t>description</t>
   </si>
@@ -8556,10 +8556,6 @@
     <t>smartspace-mutation -test-1</t>
   </si>
   <si>
-    <t>update灯
-Luminance_Setpoint</t>
-  </si>
-  <si>
     <t>mutation mutationName{
    Luminance_Setpoint_Update(input:
    [
@@ -8583,10 +8579,6 @@
     <t>smartspace-mutation -test-2</t>
   </si>
   <si>
-    <t>update 会议室模式
-Mode_Command</t>
-  </si>
-  <si>
     <t>mutation mutationName{
    Mode_Command_Update(input:
    [
@@ -8607,23 +8599,6 @@
     <t>smartspace-mutation -test-3</t>
   </si>
   <si>
-    <t>mutation mutationName{
-   Mode_Command_Update(input:
-   [
-        {
-          sourceId: "GmsDevice_1_7105_29360128.Present_Value",
-          value: "0"
-        }
-    ]
-    )
-    {
-        json_value
-        reserved_field_1
-        reserved_field_2
-    }
-}</t>
-  </si>
-  <si>
     <t>smartspace-mutation -test-4</t>
   </si>
   <si>
@@ -8651,10 +8626,6 @@
     <t>smartspace-mutation -test-5</t>
   </si>
   <si>
-    <t>update 窗帘开合度
-Position_Command</t>
-  </si>
-  <si>
     <t>mutation mutationName{
    Position_Command_Update(input:
    [
@@ -8675,10 +8646,6 @@
     <t>smartspace-mutation -test-6</t>
   </si>
   <si>
-    <t>update空调风速
-Speed_Setpoint</t>
-  </si>
-  <si>
     <t>mutation mutationName{
    Speed_Setpoint_Update(input:
    [
@@ -8694,9 +8661,6 @@
         reserved_field_2
     }
 }</t>
-  </si>
-  <si>
-    <t>smartspace-mutation -test-7</t>
   </si>
   <si>
     <t>Update空调温度
@@ -8843,6 +8807,49 @@
     }
   }
 }</t>
+  </si>
+  <si>
+    <t>Update灯
+Luminance_Setpoint</t>
+  </si>
+  <si>
+    <t>Update 会议室模式
+Mode_Command</t>
+  </si>
+  <si>
+    <t>Update 窗帘开合度
+Position_Command</t>
+  </si>
+  <si>
+    <t>Update空调风速
+Speed_Setpoint</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">获取Temperature_Sensor（室内温度℃）实时数据
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>按时间升序（captureTime ASC）排序</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Point(type='Temperature_Sensor',sourceId='')-&gt;Timeseries(captureTime)
+sourcesystem:Desigocc</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -9250,8 +9257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13585E94-2A3C-423F-8526-0CA62361FED2}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8"/>
@@ -9854,7 +9861,7 @@
         <v>81</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>725</v>
+        <v>719</v>
       </c>
       <c r="E8" s="5">
         <v>200</v>
@@ -9877,7 +9884,7 @@
         <v>81</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>726</v>
+        <v>720</v>
       </c>
       <c r="E9" s="5">
         <v>200</v>
@@ -9900,7 +9907,7 @@
         <v>81</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>727</v>
+        <v>721</v>
       </c>
       <c r="E10" s="5">
         <v>200</v>
@@ -10084,7 +10091,7 @@
         <v>81</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>728</v>
+        <v>722</v>
       </c>
       <c r="E18" s="5">
         <v>200</v>
@@ -10107,7 +10114,7 @@
         <v>81</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>729</v>
+        <v>723</v>
       </c>
       <c r="E19" s="5">
         <v>200</v>
@@ -12080,8 +12087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD19F9B6-DC75-4BF7-B9E0-0E87F10FA6D7}">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8"/>
@@ -12776,7 +12783,7 @@
         <v>576</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>577</v>
+        <v>728</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>462</v>
@@ -12808,7 +12815,7 @@
         <v>582</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>577</v>
+        <v>728</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>462</v>
@@ -13547,10 +13554,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62C1EE03-E73B-49E8-9A64-35D7806FB5EA}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8"/>
@@ -13600,13 +13607,13 @@
         <v>704</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>705</v>
+        <v>724</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>351</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E2" s="5">
         <v>200</v>
@@ -13621,21 +13628,21 @@
         <v>0</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="124.2" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>709</v>
+        <v>725</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>365</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="E3" s="5">
         <v>200</v>
@@ -13650,15 +13657,15 @@
         <v>0</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="124.2" customHeight="1">
       <c r="A4" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>711</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>709</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>365</v>
@@ -13679,21 +13686,21 @@
         <v>0</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="124.2" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>726</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>714</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>365</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>715</v>
       </c>
       <c r="E5" s="5">
         <v>200</v>
@@ -13708,21 +13715,21 @@
         <v>0</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="124.2" customHeight="1">
       <c r="A6" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>727</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>716</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>717</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>718</v>
       </c>
       <c r="E6" s="5">
         <v>200</v>
@@ -13737,21 +13744,21 @@
         <v>0</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="124.2" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>337</v>
+        <v>323</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
       <c r="E7" s="5">
         <v>200</v>
@@ -13766,39 +13773,11 @@
         <v>0</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="124.2" customHeight="1">
-      <c r="A8" s="1" t="s">
-        <v>722</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>723</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>323</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>724</v>
-      </c>
-      <c r="E8" s="5">
-        <v>200</v>
-      </c>
-      <c r="F8" s="5">
-        <v>100000</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8" s="1">
-        <v>0</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>